<commit_message>
Criação do roteiro de confirmação de reserva
</commit_message>
<xml_diff>
--- a/Confirmação de Reserva/Confirmação de reserva.xlsx
+++ b/Confirmação de Reserva/Confirmação de reserva.xlsx
@@ -19185,8 +19185,8 @@
   </sheetPr>
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" zoomScale="90" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A7" zoomScale="90" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>

</xml_diff>